<commit_message>
Updated bug tracker with fixes from previous commit
</commit_message>
<xml_diff>
--- a/pc_lock_test/PC Break Timer Bug Tracker.xlsx
+++ b/pc_lock_test/PC Break Timer Bug Tracker.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
   <si>
     <t>Type</t>
   </si>
@@ -252,6 +252,9 @@
   </si>
   <si>
     <t>Message box caption text indented too far</t>
+  </si>
+  <si>
+    <t>V0.10.1</t>
   </si>
 </sst>
 </file>
@@ -1012,8 +1015,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="115853568"/>
-        <c:axId val="115748864"/>
+        <c:axId val="108321024"/>
+        <c:axId val="108736512"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -2824,11 +2827,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="115853568"/>
-        <c:axId val="115748864"/>
+        <c:axId val="108321024"/>
+        <c:axId val="108736512"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="115853568"/>
+        <c:axId val="108321024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2876,14 +2879,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="115748864"/>
+        <c:crossAx val="108736512"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="115748864"/>
+        <c:axId val="108736512"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2893,7 +2896,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="115853568"/>
+        <c:crossAx val="108321024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3902,7 +3905,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3917,7 +3920,7 @@
   <dimension ref="B1:N201"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4152,9 +4155,15 @@
       <c r="G18" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H18" s="3"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="20"/>
+      <c r="H18" s="3">
+        <v>42774</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J18" s="20" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="19" spans="2:14" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
@@ -4175,9 +4184,15 @@
       <c r="G19" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H19" s="3"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="20"/>
+      <c r="H19" s="3">
+        <v>42774</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J19" s="20" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="20" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B20" s="2">

</xml_diff>

<commit_message>
V0.10.3 - Bug fix Reverted to old method of preventing locking
This may or may not work, requires further Alpha testing at work and home
to determin if it is a code problem or PC setting problem. Could not
reproduce the bug where the time until home counter would be wrong on
Friday's. Should fix loading mouse over bug (not documented).
</commit_message>
<xml_diff>
--- a/pc_lock_test/PC Break Timer Bug Tracker.xlsx
+++ b/pc_lock_test/PC Break Timer Bug Tracker.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
   <si>
     <t>Type</t>
   </si>
@@ -257,13 +257,13 @@
     <t>V0.10.1</t>
   </si>
   <si>
-    <t>Time to hoem timer wrong on shoter work days</t>
-  </si>
-  <si>
     <t>Relibilirt</t>
   </si>
   <si>
-    <t>Home time is still correct</t>
+    <t>Time to home timer wrong on shoter work days</t>
+  </si>
+  <si>
+    <t>Could not reproduce</t>
   </si>
 </sst>
 </file>
@@ -818,97 +818,97 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>2</c:v>
@@ -1024,8 +1024,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="46729472"/>
-        <c:axId val="46743552"/>
+        <c:axId val="108931328"/>
+        <c:axId val="108941312"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1066,199 +1066,199 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>42743</c:v>
+                  <c:v>42774</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42744</c:v>
+                  <c:v>42775</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42745</c:v>
+                  <c:v>42776</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42746</c:v>
+                  <c:v>42777</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42747</c:v>
+                  <c:v>42778</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42748</c:v>
+                  <c:v>42779</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42749</c:v>
+                  <c:v>42780</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42750</c:v>
+                  <c:v>42781</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42751</c:v>
+                  <c:v>42782</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42752</c:v>
+                  <c:v>42783</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42753</c:v>
+                  <c:v>42784</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42754</c:v>
+                  <c:v>42785</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42755</c:v>
+                  <c:v>42786</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42756</c:v>
+                  <c:v>42787</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>42757</c:v>
+                  <c:v>42788</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42758</c:v>
+                  <c:v>42789</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>42759</c:v>
+                  <c:v>42790</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>42760</c:v>
+                  <c:v>42791</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>42761</c:v>
+                  <c:v>42792</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>42762</c:v>
+                  <c:v>42793</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>42763</c:v>
+                  <c:v>42794</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>42764</c:v>
+                  <c:v>42795</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>42765</c:v>
+                  <c:v>42796</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>42766</c:v>
+                  <c:v>42797</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>42767</c:v>
+                  <c:v>42798</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>42768</c:v>
+                  <c:v>42799</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>42769</c:v>
+                  <c:v>42800</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>42770</c:v>
+                  <c:v>42801</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>42771</c:v>
+                  <c:v>42802</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>42772</c:v>
+                  <c:v>42803</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>42773</c:v>
+                  <c:v>42804</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>42774</c:v>
+                  <c:v>42805</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>42775</c:v>
+                  <c:v>42806</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>42776</c:v>
+                  <c:v>42807</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>42777</c:v>
+                  <c:v>42808</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>42778</c:v>
+                  <c:v>42809</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>42779</c:v>
+                  <c:v>42810</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>42780</c:v>
+                  <c:v>42811</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>42781</c:v>
+                  <c:v>42812</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>42782</c:v>
+                  <c:v>42813</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>42783</c:v>
+                  <c:v>42814</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>42784</c:v>
+                  <c:v>42815</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>42785</c:v>
+                  <c:v>42816</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>42786</c:v>
+                  <c:v>42817</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>42787</c:v>
+                  <c:v>42818</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>42788</c:v>
+                  <c:v>42819</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>42789</c:v>
+                  <c:v>42820</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>42790</c:v>
+                  <c:v>42821</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>42791</c:v>
+                  <c:v>42822</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>42792</c:v>
+                  <c:v>42823</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>42793</c:v>
+                  <c:v>42824</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>42794</c:v>
+                  <c:v>42825</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>42795</c:v>
+                  <c:v>42826</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>42796</c:v>
+                  <c:v>42827</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>42797</c:v>
+                  <c:v>42828</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>42798</c:v>
+                  <c:v>42829</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>42799</c:v>
+                  <c:v>42830</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>42800</c:v>
+                  <c:v>42831</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>42801</c:v>
+                  <c:v>42832</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>42802</c:v>
+                  <c:v>42833</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>42803</c:v>
+                  <c:v>42834</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>42804</c:v>
+                  <c:v>42835</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>42805</c:v>
+                  <c:v>42836</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>42806</c:v>
+                  <c:v>42837</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>42807</c:v>
+                  <c:v>42838</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1270,97 +1270,97 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>2</c:v>
@@ -1444,25 +1444,25 @@
                   <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1513,199 +1513,199 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>42743</c:v>
+                  <c:v>42774</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42744</c:v>
+                  <c:v>42775</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42745</c:v>
+                  <c:v>42776</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42746</c:v>
+                  <c:v>42777</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42747</c:v>
+                  <c:v>42778</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42748</c:v>
+                  <c:v>42779</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42749</c:v>
+                  <c:v>42780</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42750</c:v>
+                  <c:v>42781</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42751</c:v>
+                  <c:v>42782</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42752</c:v>
+                  <c:v>42783</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42753</c:v>
+                  <c:v>42784</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42754</c:v>
+                  <c:v>42785</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42755</c:v>
+                  <c:v>42786</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42756</c:v>
+                  <c:v>42787</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>42757</c:v>
+                  <c:v>42788</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42758</c:v>
+                  <c:v>42789</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>42759</c:v>
+                  <c:v>42790</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>42760</c:v>
+                  <c:v>42791</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>42761</c:v>
+                  <c:v>42792</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>42762</c:v>
+                  <c:v>42793</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>42763</c:v>
+                  <c:v>42794</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>42764</c:v>
+                  <c:v>42795</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>42765</c:v>
+                  <c:v>42796</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>42766</c:v>
+                  <c:v>42797</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>42767</c:v>
+                  <c:v>42798</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>42768</c:v>
+                  <c:v>42799</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>42769</c:v>
+                  <c:v>42800</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>42770</c:v>
+                  <c:v>42801</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>42771</c:v>
+                  <c:v>42802</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>42772</c:v>
+                  <c:v>42803</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>42773</c:v>
+                  <c:v>42804</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>42774</c:v>
+                  <c:v>42805</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>42775</c:v>
+                  <c:v>42806</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>42776</c:v>
+                  <c:v>42807</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>42777</c:v>
+                  <c:v>42808</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>42778</c:v>
+                  <c:v>42809</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>42779</c:v>
+                  <c:v>42810</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>42780</c:v>
+                  <c:v>42811</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>42781</c:v>
+                  <c:v>42812</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>42782</c:v>
+                  <c:v>42813</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>42783</c:v>
+                  <c:v>42814</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>42784</c:v>
+                  <c:v>42815</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>42785</c:v>
+                  <c:v>42816</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>42786</c:v>
+                  <c:v>42817</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>42787</c:v>
+                  <c:v>42818</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>42788</c:v>
+                  <c:v>42819</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>42789</c:v>
+                  <c:v>42820</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>42790</c:v>
+                  <c:v>42821</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>42791</c:v>
+                  <c:v>42822</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>42792</c:v>
+                  <c:v>42823</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>42793</c:v>
+                  <c:v>42824</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>42794</c:v>
+                  <c:v>42825</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>42795</c:v>
+                  <c:v>42826</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>42796</c:v>
+                  <c:v>42827</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>42797</c:v>
+                  <c:v>42828</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>42798</c:v>
+                  <c:v>42829</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>42799</c:v>
+                  <c:v>42830</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>42800</c:v>
+                  <c:v>42831</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>42801</c:v>
+                  <c:v>42832</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>42802</c:v>
+                  <c:v>42833</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>42803</c:v>
+                  <c:v>42834</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>42804</c:v>
+                  <c:v>42835</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>42805</c:v>
+                  <c:v>42836</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>42806</c:v>
+                  <c:v>42837</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>42807</c:v>
+                  <c:v>42838</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1717,97 +1717,97 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="31">
                   <c:v>2</c:v>
@@ -1995,199 +1995,199 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>42743</c:v>
+                  <c:v>42774</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42744</c:v>
+                  <c:v>42775</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42745</c:v>
+                  <c:v>42776</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42746</c:v>
+                  <c:v>42777</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42747</c:v>
+                  <c:v>42778</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42748</c:v>
+                  <c:v>42779</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42749</c:v>
+                  <c:v>42780</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42750</c:v>
+                  <c:v>42781</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42751</c:v>
+                  <c:v>42782</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42752</c:v>
+                  <c:v>42783</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42753</c:v>
+                  <c:v>42784</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42754</c:v>
+                  <c:v>42785</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42755</c:v>
+                  <c:v>42786</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42756</c:v>
+                  <c:v>42787</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>42757</c:v>
+                  <c:v>42788</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42758</c:v>
+                  <c:v>42789</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>42759</c:v>
+                  <c:v>42790</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>42760</c:v>
+                  <c:v>42791</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>42761</c:v>
+                  <c:v>42792</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>42762</c:v>
+                  <c:v>42793</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>42763</c:v>
+                  <c:v>42794</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>42764</c:v>
+                  <c:v>42795</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>42765</c:v>
+                  <c:v>42796</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>42766</c:v>
+                  <c:v>42797</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>42767</c:v>
+                  <c:v>42798</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>42768</c:v>
+                  <c:v>42799</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>42769</c:v>
+                  <c:v>42800</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>42770</c:v>
+                  <c:v>42801</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>42771</c:v>
+                  <c:v>42802</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>42772</c:v>
+                  <c:v>42803</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>42773</c:v>
+                  <c:v>42804</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>42774</c:v>
+                  <c:v>42805</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>42775</c:v>
+                  <c:v>42806</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>42776</c:v>
+                  <c:v>42807</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>42777</c:v>
+                  <c:v>42808</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>42778</c:v>
+                  <c:v>42809</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>42779</c:v>
+                  <c:v>42810</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>42780</c:v>
+                  <c:v>42811</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>42781</c:v>
+                  <c:v>42812</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>42782</c:v>
+                  <c:v>42813</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>42783</c:v>
+                  <c:v>42814</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>42784</c:v>
+                  <c:v>42815</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>42785</c:v>
+                  <c:v>42816</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>42786</c:v>
+                  <c:v>42817</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>42787</c:v>
+                  <c:v>42818</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>42788</c:v>
+                  <c:v>42819</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>42789</c:v>
+                  <c:v>42820</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>42790</c:v>
+                  <c:v>42821</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>42791</c:v>
+                  <c:v>42822</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>42792</c:v>
+                  <c:v>42823</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>42793</c:v>
+                  <c:v>42824</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>42794</c:v>
+                  <c:v>42825</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>42795</c:v>
+                  <c:v>42826</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>42796</c:v>
+                  <c:v>42827</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>42797</c:v>
+                  <c:v>42828</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>42798</c:v>
+                  <c:v>42829</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>42799</c:v>
+                  <c:v>42830</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>42800</c:v>
+                  <c:v>42831</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>42801</c:v>
+                  <c:v>42832</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>42802</c:v>
+                  <c:v>42833</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>42803</c:v>
+                  <c:v>42834</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>42804</c:v>
+                  <c:v>42835</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>42805</c:v>
+                  <c:v>42836</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>42806</c:v>
+                  <c:v>42837</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>42807</c:v>
+                  <c:v>42838</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2199,274 +2199,274 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2.08</c:v>
+                  <c:v>3.12</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2.08</c:v>
+                  <c:v>3.12</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2.08</c:v>
+                  <c:v>3.12</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>2.08</c:v>
+                  <c:v>3.12</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2.08</c:v>
+                  <c:v>3.12</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2.08</c:v>
+                  <c:v>3.12</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2.08</c:v>
+                  <c:v>3.12</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2552,274 +2552,274 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2.08</c:v>
+                  <c:v>2.12</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.08</c:v>
+                  <c:v>0.12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2836,11 +2836,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="46729472"/>
-        <c:axId val="46743552"/>
+        <c:axId val="108931328"/>
+        <c:axId val="108941312"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="46729472"/>
+        <c:axId val="108931328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2888,14 +2888,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="46743552"/>
+        <c:crossAx val="108941312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="46743552"/>
+        <c:axId val="108941312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2905,7 +2905,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="46729472"/>
+        <c:crossAx val="108931328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3928,7 +3928,7 @@
   </sheetPr>
   <dimension ref="B1:N201"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -3994,7 +3994,7 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">TODAY()</f>
-        <v>42832</v>
+        <v>42863</v>
       </c>
       <c r="J3" s="8">
         <v>90</v>
@@ -4208,10 +4208,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D20" s="12" t="s">
         <v>58</v>
-      </c>
-      <c r="D20" s="12" t="s">
-        <v>59</v>
       </c>
       <c r="E20" s="22" t="s">
         <v>30</v>
@@ -4222,8 +4222,12 @@
       <c r="G20" s="12" t="s">
         <v>54</v>
       </c>
-      <c r="H20" s="3"/>
-      <c r="I20" s="2"/>
+      <c r="H20" s="3">
+        <v>42863</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="J20" s="20" t="s">
         <v>60</v>
       </c>
@@ -5107,7 +5111,7 @@
       </c>
       <c r="J8" s="1">
         <f ca="1">'Issue Tracker'!I3</f>
-        <v>42832</v>
+        <v>42863</v>
       </c>
       <c r="N8">
         <f ca="1">COUNT(typesUnsorted)</f>
@@ -5195,15 +5199,15 @@
       </c>
       <c r="H16" s="1">
         <f t="shared" ref="H16:H47" ca="1" si="0">keydate-days+G16</f>
-        <v>42743</v>
+        <v>42774</v>
       </c>
       <c r="I16">
         <f ca="1">I15+COUNTIFS(issues[OPENED ON],H16,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J16">
         <f ca="1">J15+COUNTIFS(issues[CLOSED ON],H16,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N16" t="str">
         <f t="array" ref="N16">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N15, issues[TYPE]),0))</f>
@@ -5228,15 +5232,15 @@
       </c>
       <c r="H17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42744</v>
+        <v>42775</v>
       </c>
       <c r="I17">
         <f ca="1">I16+COUNTIFS(issues[OPENED ON],H17,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J17">
         <f ca="1">J16+COUNTIFS(issues[CLOSED ON],H17,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N17" t="str">
         <f t="array" ref="N17">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N16, issues[TYPE]),0))</f>
@@ -5261,15 +5265,15 @@
       </c>
       <c r="H18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42745</v>
+        <v>42776</v>
       </c>
       <c r="I18">
         <f ca="1">I17+COUNTIFS(issues[OPENED ON],H18,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J18">
         <f ca="1">J17+COUNTIFS(issues[CLOSED ON],H18,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N18">
         <f t="array" ref="N18">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N17, issues[TYPE]),0))</f>
@@ -5294,15 +5298,15 @@
       </c>
       <c r="H19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42746</v>
+        <v>42777</v>
       </c>
       <c r="I19">
         <f ca="1">I18+COUNTIFS(issues[OPENED ON],H19,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J19">
         <f ca="1">J18+COUNTIFS(issues[CLOSED ON],H19,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N19" t="e">
         <f t="array" ref="N19">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N18, issues[TYPE]),0))</f>
@@ -5327,15 +5331,15 @@
       </c>
       <c r="H20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42747</v>
+        <v>42778</v>
       </c>
       <c r="I20">
         <f ca="1">I19+COUNTIFS(issues[OPENED ON],H20,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J20">
         <f ca="1">J19+COUNTIFS(issues[CLOSED ON],H20,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N20" t="e">
         <f t="array" ref="N20">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N19, issues[TYPE]),0))</f>
@@ -5360,15 +5364,15 @@
       </c>
       <c r="H21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42748</v>
+        <v>42779</v>
       </c>
       <c r="I21">
         <f ca="1">I20+COUNTIFS(issues[OPENED ON],H21,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J21">
         <f ca="1">J20+COUNTIFS(issues[CLOSED ON],H21,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N21" t="e">
         <f t="array" ref="N21">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N20, issues[TYPE]),0))</f>
@@ -5393,15 +5397,15 @@
       </c>
       <c r="H22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42749</v>
+        <v>42780</v>
       </c>
       <c r="I22">
         <f ca="1">I21+COUNTIFS(issues[OPENED ON],H22,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J22">
         <f ca="1">J21+COUNTIFS(issues[CLOSED ON],H22,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N22" t="e">
         <f t="array" ref="N22">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N21, issues[TYPE]),0))</f>
@@ -5426,15 +5430,15 @@
       </c>
       <c r="H23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42750</v>
+        <v>42781</v>
       </c>
       <c r="I23">
         <f ca="1">I22+COUNTIFS(issues[OPENED ON],H23,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J23">
         <f ca="1">J22+COUNTIFS(issues[CLOSED ON],H23,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N23" t="e">
         <f t="array" ref="N23">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N22, issues[TYPE]),0))</f>
@@ -5459,15 +5463,15 @@
       </c>
       <c r="H24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42751</v>
+        <v>42782</v>
       </c>
       <c r="I24">
         <f ca="1">I23+COUNTIFS(issues[OPENED ON],H24,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J24">
         <f ca="1">J23+COUNTIFS(issues[CLOSED ON],H24,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N24" t="e">
         <f t="array" ref="N24">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N23, issues[TYPE]),0))</f>
@@ -5492,15 +5496,15 @@
       </c>
       <c r="H25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42752</v>
+        <v>42783</v>
       </c>
       <c r="I25">
         <f ca="1">I24+COUNTIFS(issues[OPENED ON],H25,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J25">
         <f ca="1">J24+COUNTIFS(issues[CLOSED ON],H25,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N25" t="e">
         <f t="array" ref="N25">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N24, issues[TYPE]),0))</f>
@@ -5525,15 +5529,15 @@
       </c>
       <c r="H26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42753</v>
+        <v>42784</v>
       </c>
       <c r="I26">
         <f ca="1">I25+COUNTIFS(issues[OPENED ON],H26,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J26">
         <f ca="1">J25+COUNTIFS(issues[CLOSED ON],H26,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N26" t="e">
         <f t="array" ref="N26">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N25, issues[TYPE]),0))</f>
@@ -5558,15 +5562,15 @@
       </c>
       <c r="H27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42754</v>
+        <v>42785</v>
       </c>
       <c r="I27">
         <f ca="1">I26+COUNTIFS(issues[OPENED ON],H27,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J27">
         <f ca="1">J26+COUNTIFS(issues[CLOSED ON],H27,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N27" t="e">
         <f t="array" ref="N27">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N26, issues[TYPE]),0))</f>
@@ -5591,15 +5595,15 @@
       </c>
       <c r="H28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42755</v>
+        <v>42786</v>
       </c>
       <c r="I28">
         <f ca="1">I27+COUNTIFS(issues[OPENED ON],H28,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J28">
         <f ca="1">J27+COUNTIFS(issues[CLOSED ON],H28,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N28" t="e">
         <f t="array" ref="N28">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N27, issues[TYPE]),0))</f>
@@ -5624,15 +5628,15 @@
       </c>
       <c r="H29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42756</v>
+        <v>42787</v>
       </c>
       <c r="I29">
         <f ca="1">I28+COUNTIFS(issues[OPENED ON],H29,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J29">
         <f ca="1">J28+COUNTIFS(issues[CLOSED ON],H29,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N29" t="e">
         <f t="array" ref="N29">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N28, issues[TYPE]),0))</f>
@@ -5657,15 +5661,15 @@
       </c>
       <c r="H30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42757</v>
+        <v>42788</v>
       </c>
       <c r="I30">
         <f ca="1">I29+COUNTIFS(issues[OPENED ON],H30,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J30">
         <f ca="1">J29+COUNTIFS(issues[CLOSED ON],H30,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N30" t="e">
         <f t="array" ref="N30">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N29, issues[TYPE]),0))</f>
@@ -5690,15 +5694,15 @@
       </c>
       <c r="H31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42758</v>
+        <v>42789</v>
       </c>
       <c r="I31">
         <f ca="1">I30+COUNTIFS(issues[OPENED ON],H31,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J31">
         <f ca="1">J30+COUNTIFS(issues[CLOSED ON],H31,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N31" t="e">
         <f t="array" ref="N31">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N30, issues[TYPE]),0))</f>
@@ -5723,15 +5727,15 @@
       </c>
       <c r="H32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42759</v>
+        <v>42790</v>
       </c>
       <c r="I32">
         <f ca="1">I31+COUNTIFS(issues[OPENED ON],H32,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J32">
         <f ca="1">J31+COUNTIFS(issues[CLOSED ON],H32,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N32" t="e">
         <f t="array" ref="N32">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N31, issues[TYPE]),0))</f>
@@ -5756,15 +5760,15 @@
       </c>
       <c r="H33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42760</v>
+        <v>42791</v>
       </c>
       <c r="I33">
         <f ca="1">I32+COUNTIFS(issues[OPENED ON],H33,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J33">
         <f ca="1">J32+COUNTIFS(issues[CLOSED ON],H33,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N33" t="e">
         <f t="array" ref="N33">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N32, issues[TYPE]),0))</f>
@@ -5789,15 +5793,15 @@
       </c>
       <c r="H34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42761</v>
+        <v>42792</v>
       </c>
       <c r="I34">
         <f ca="1">I33+COUNTIFS(issues[OPENED ON],H34,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J34">
         <f ca="1">J33+COUNTIFS(issues[CLOSED ON],H34,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N34" t="e">
         <f t="array" ref="N34">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N33, issues[TYPE]),0))</f>
@@ -5822,15 +5826,15 @@
       </c>
       <c r="H35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42762</v>
+        <v>42793</v>
       </c>
       <c r="I35">
         <f ca="1">I34+COUNTIFS(issues[OPENED ON],H35,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J35">
         <f ca="1">J34+COUNTIFS(issues[CLOSED ON],H35,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N35" t="e">
         <f t="array" ref="N35">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N34, issues[TYPE]),0))</f>
@@ -5855,15 +5859,15 @@
       </c>
       <c r="H36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42763</v>
+        <v>42794</v>
       </c>
       <c r="I36">
         <f ca="1">I35+COUNTIFS(issues[OPENED ON],H36,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J36">
         <f ca="1">J35+COUNTIFS(issues[CLOSED ON],H36,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N36" t="e">
         <f t="array" ref="N36">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N35, issues[TYPE]),0))</f>
@@ -5888,15 +5892,15 @@
       </c>
       <c r="H37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42764</v>
+        <v>42795</v>
       </c>
       <c r="I37">
         <f ca="1">I36+COUNTIFS(issues[OPENED ON],H37,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J37">
         <f ca="1">J36+COUNTIFS(issues[CLOSED ON],H37,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N37" t="e">
         <f t="array" ref="N37">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N36, issues[TYPE]),0))</f>
@@ -5921,15 +5925,15 @@
       </c>
       <c r="H38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42765</v>
+        <v>42796</v>
       </c>
       <c r="I38">
         <f ca="1">I37+COUNTIFS(issues[OPENED ON],H38,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J38">
         <f ca="1">J37+COUNTIFS(issues[CLOSED ON],H38,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N38" t="e">
         <f t="array" ref="N38">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N37, issues[TYPE]),0))</f>
@@ -5954,15 +5958,15 @@
       </c>
       <c r="H39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42766</v>
+        <v>42797</v>
       </c>
       <c r="I39">
         <f ca="1">I38+COUNTIFS(issues[OPENED ON],H39,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J39">
         <f ca="1">J38+COUNTIFS(issues[CLOSED ON],H39,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N39" t="e">
         <f t="array" ref="N39">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N38, issues[TYPE]),0))</f>
@@ -5987,15 +5991,15 @@
       </c>
       <c r="H40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42767</v>
+        <v>42798</v>
       </c>
       <c r="I40">
         <f ca="1">I39+COUNTIFS(issues[OPENED ON],H40,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J40">
         <f ca="1">J39+COUNTIFS(issues[CLOSED ON],H40,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N40" t="e">
         <f t="array" ref="N40">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N39, issues[TYPE]),0))</f>
@@ -6020,15 +6024,15 @@
       </c>
       <c r="H41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42768</v>
+        <v>42799</v>
       </c>
       <c r="I41">
         <f ca="1">I40+COUNTIFS(issues[OPENED ON],H41,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J41">
         <f ca="1">J40+COUNTIFS(issues[CLOSED ON],H41,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N41" t="e">
         <f t="array" ref="N41">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N40, issues[TYPE]),0))</f>
@@ -6053,15 +6057,15 @@
       </c>
       <c r="H42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42769</v>
+        <v>42800</v>
       </c>
       <c r="I42">
         <f ca="1">I41+COUNTIFS(issues[OPENED ON],H42,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J42">
         <f ca="1">J41+COUNTIFS(issues[CLOSED ON],H42,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N42" t="e">
         <f t="array" ref="N42">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N41, issues[TYPE]),0))</f>
@@ -6086,15 +6090,15 @@
       </c>
       <c r="H43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42770</v>
+        <v>42801</v>
       </c>
       <c r="I43">
         <f ca="1">I42+COUNTIFS(issues[OPENED ON],H43,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J43">
         <f ca="1">J42+COUNTIFS(issues[CLOSED ON],H43,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N43" t="e">
         <f t="array" ref="N43">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N42, issues[TYPE]),0))</f>
@@ -6119,15 +6123,15 @@
       </c>
       <c r="H44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42771</v>
+        <v>42802</v>
       </c>
       <c r="I44">
         <f ca="1">I43+COUNTIFS(issues[OPENED ON],H44,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J44">
         <f ca="1">J43+COUNTIFS(issues[CLOSED ON],H44,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N44" t="e">
         <f t="array" ref="N44">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N43, issues[TYPE]),0))</f>
@@ -6152,15 +6156,15 @@
       </c>
       <c r="H45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42772</v>
+        <v>42803</v>
       </c>
       <c r="I45">
         <f ca="1">I44+COUNTIFS(issues[OPENED ON],H45,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J45">
         <f ca="1">J44+COUNTIFS(issues[CLOSED ON],H45,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="N45" t="e">
         <f t="array" ref="N45">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N44, issues[TYPE]),0))</f>
@@ -6185,15 +6189,15 @@
       </c>
       <c r="H46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42773</v>
+        <v>42804</v>
       </c>
       <c r="I46">
         <f ca="1">I45+COUNTIFS(issues[OPENED ON],H46,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J46">
         <f ca="1">J45+COUNTIFS(issues[CLOSED ON],H46,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="47" spans="7:20" x14ac:dyDescent="0.25">
@@ -6202,7 +6206,7 @@
       </c>
       <c r="H47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42774</v>
+        <v>42805</v>
       </c>
       <c r="I47">
         <f ca="1">I46+COUNTIFS(issues[OPENED ON],H47,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6219,7 +6223,7 @@
       </c>
       <c r="H48" s="1">
         <f t="shared" ref="H48:H79" ca="1" si="1">keydate-days+G48</f>
-        <v>42775</v>
+        <v>42806</v>
       </c>
       <c r="I48">
         <f ca="1">I47+COUNTIFS(issues[OPENED ON],H48,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6236,7 +6240,7 @@
       </c>
       <c r="H49" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42776</v>
+        <v>42807</v>
       </c>
       <c r="I49">
         <f ca="1">I48+COUNTIFS(issues[OPENED ON],H49,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6253,7 +6257,7 @@
       </c>
       <c r="H50" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42777</v>
+        <v>42808</v>
       </c>
       <c r="I50">
         <f ca="1">I49+COUNTIFS(issues[OPENED ON],H50,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6270,7 +6274,7 @@
       </c>
       <c r="H51" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42778</v>
+        <v>42809</v>
       </c>
       <c r="I51">
         <f ca="1">I50+COUNTIFS(issues[OPENED ON],H51,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6287,7 +6291,7 @@
       </c>
       <c r="H52" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42779</v>
+        <v>42810</v>
       </c>
       <c r="I52">
         <f ca="1">I51+COUNTIFS(issues[OPENED ON],H52,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6304,7 +6308,7 @@
       </c>
       <c r="H53" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42780</v>
+        <v>42811</v>
       </c>
       <c r="I53">
         <f ca="1">I52+COUNTIFS(issues[OPENED ON],H53,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6321,7 +6325,7 @@
       </c>
       <c r="H54" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42781</v>
+        <v>42812</v>
       </c>
       <c r="I54">
         <f ca="1">I53+COUNTIFS(issues[OPENED ON],H54,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6338,7 +6342,7 @@
       </c>
       <c r="H55" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42782</v>
+        <v>42813</v>
       </c>
       <c r="I55">
         <f ca="1">I54+COUNTIFS(issues[OPENED ON],H55,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6355,7 +6359,7 @@
       </c>
       <c r="H56" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42783</v>
+        <v>42814</v>
       </c>
       <c r="I56">
         <f ca="1">I55+COUNTIFS(issues[OPENED ON],H56,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6372,7 +6376,7 @@
       </c>
       <c r="H57" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42784</v>
+        <v>42815</v>
       </c>
       <c r="I57">
         <f ca="1">I56+COUNTIFS(issues[OPENED ON],H57,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6389,7 +6393,7 @@
       </c>
       <c r="H58" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42785</v>
+        <v>42816</v>
       </c>
       <c r="I58">
         <f ca="1">I57+COUNTIFS(issues[OPENED ON],H58,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6406,7 +6410,7 @@
       </c>
       <c r="H59" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42786</v>
+        <v>42817</v>
       </c>
       <c r="I59">
         <f ca="1">I58+COUNTIFS(issues[OPENED ON],H59,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6423,7 +6427,7 @@
       </c>
       <c r="H60" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42787</v>
+        <v>42818</v>
       </c>
       <c r="I60">
         <f ca="1">I59+COUNTIFS(issues[OPENED ON],H60,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6440,7 +6444,7 @@
       </c>
       <c r="H61" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42788</v>
+        <v>42819</v>
       </c>
       <c r="I61">
         <f ca="1">I60+COUNTIFS(issues[OPENED ON],H61,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6457,7 +6461,7 @@
       </c>
       <c r="H62" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42789</v>
+        <v>42820</v>
       </c>
       <c r="I62">
         <f ca="1">I61+COUNTIFS(issues[OPENED ON],H62,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6474,7 +6478,7 @@
       </c>
       <c r="H63" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42790</v>
+        <v>42821</v>
       </c>
       <c r="I63">
         <f ca="1">I62+COUNTIFS(issues[OPENED ON],H63,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6491,7 +6495,7 @@
       </c>
       <c r="H64" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42791</v>
+        <v>42822</v>
       </c>
       <c r="I64">
         <f ca="1">I63+COUNTIFS(issues[OPENED ON],H64,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6508,7 +6512,7 @@
       </c>
       <c r="H65" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42792</v>
+        <v>42823</v>
       </c>
       <c r="I65">
         <f ca="1">I64+COUNTIFS(issues[OPENED ON],H65,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6525,7 +6529,7 @@
       </c>
       <c r="H66" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42793</v>
+        <v>42824</v>
       </c>
       <c r="I66">
         <f ca="1">I65+COUNTIFS(issues[OPENED ON],H66,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6542,7 +6546,7 @@
       </c>
       <c r="H67" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42794</v>
+        <v>42825</v>
       </c>
       <c r="I67">
         <f ca="1">I66+COUNTIFS(issues[OPENED ON],H67,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6559,7 +6563,7 @@
       </c>
       <c r="H68" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42795</v>
+        <v>42826</v>
       </c>
       <c r="I68">
         <f ca="1">I67+COUNTIFS(issues[OPENED ON],H68,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6576,7 +6580,7 @@
       </c>
       <c r="H69" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42796</v>
+        <v>42827</v>
       </c>
       <c r="I69">
         <f ca="1">I68+COUNTIFS(issues[OPENED ON],H69,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6593,7 +6597,7 @@
       </c>
       <c r="H70" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42797</v>
+        <v>42828</v>
       </c>
       <c r="I70">
         <f ca="1">I69+COUNTIFS(issues[OPENED ON],H70,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6610,7 +6614,7 @@
       </c>
       <c r="H71" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42798</v>
+        <v>42829</v>
       </c>
       <c r="I71">
         <f ca="1">I70+COUNTIFS(issues[OPENED ON],H71,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6627,7 +6631,7 @@
       </c>
       <c r="H72" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42799</v>
+        <v>42830</v>
       </c>
       <c r="I72">
         <f ca="1">I71+COUNTIFS(issues[OPENED ON],H72,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6644,7 +6648,7 @@
       </c>
       <c r="H73" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42800</v>
+        <v>42831</v>
       </c>
       <c r="I73">
         <f ca="1">I72+COUNTIFS(issues[OPENED ON],H73,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6661,11 +6665,11 @@
       </c>
       <c r="H74" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42801</v>
+        <v>42832</v>
       </c>
       <c r="I74">
         <f ca="1">I73+COUNTIFS(issues[OPENED ON],H74,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J74">
         <f ca="1">J73+COUNTIFS(issues[CLOSED ON],H74,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6678,11 +6682,11 @@
       </c>
       <c r="H75" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42802</v>
+        <v>42833</v>
       </c>
       <c r="I75">
         <f ca="1">I74+COUNTIFS(issues[OPENED ON],H75,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J75">
         <f ca="1">J74+COUNTIFS(issues[CLOSED ON],H75,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6695,11 +6699,11 @@
       </c>
       <c r="H76" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42803</v>
+        <v>42834</v>
       </c>
       <c r="I76">
         <f ca="1">I75+COUNTIFS(issues[OPENED ON],H76,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J76">
         <f ca="1">J75+COUNTIFS(issues[CLOSED ON],H76,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6712,11 +6716,11 @@
       </c>
       <c r="H77" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42804</v>
+        <v>42835</v>
       </c>
       <c r="I77">
         <f ca="1">I76+COUNTIFS(issues[OPENED ON],H77,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J77">
         <f ca="1">J76+COUNTIFS(issues[CLOSED ON],H77,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6729,11 +6733,11 @@
       </c>
       <c r="H78" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42805</v>
+        <v>42836</v>
       </c>
       <c r="I78">
         <f ca="1">I77+COUNTIFS(issues[OPENED ON],H78,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J78">
         <f ca="1">J77+COUNTIFS(issues[CLOSED ON],H78,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6746,11 +6750,11 @@
       </c>
       <c r="H79" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42806</v>
+        <v>42837</v>
       </c>
       <c r="I79">
         <f ca="1">I78+COUNTIFS(issues[OPENED ON],H79,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J79">
         <f ca="1">J78+COUNTIFS(issues[CLOSED ON],H79,issues[TYPE],type,issues[PRIORITY],priority)</f>
@@ -6763,11 +6767,11 @@
       </c>
       <c r="H80" s="1">
         <f t="shared" ref="H80" ca="1" si="2">keydate-days+G80</f>
-        <v>42807</v>
+        <v>42838</v>
       </c>
       <c r="I80">
         <f ca="1">I79+COUNTIFS(issues[OPENED ON],H80,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="J80">
         <f ca="1">J79+COUNTIFS(issues[CLOSED ON],H80,issues[TYPE],type,issues[PRIORITY],priority)</f>

</xml_diff>

<commit_message>
Fixed typo in bug tracker
</commit_message>
<xml_diff>
--- a/pc_lock_test/PC Break Timer Bug Tracker.xlsx
+++ b/pc_lock_test/PC Break Timer Bug Tracker.xlsx
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="60">
   <si>
     <t>Type</t>
   </si>
@@ -255,9 +255,6 @@
   </si>
   <si>
     <t>V0.10.1</t>
-  </si>
-  <si>
-    <t>Relibilirt</t>
   </si>
   <si>
     <t>Time to home timer wrong on shoter work days</t>
@@ -818,199 +815,199 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1024,8 +1021,8 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="108931328"/>
-        <c:axId val="108941312"/>
+        <c:axId val="77420800"/>
+        <c:axId val="77434880"/>
       </c:areaChart>
       <c:lineChart>
         <c:grouping val="standard"/>
@@ -1066,199 +1063,199 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>42774</c:v>
+                  <c:v>42804</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42775</c:v>
+                  <c:v>42805</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42776</c:v>
+                  <c:v>42806</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42777</c:v>
+                  <c:v>42807</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42778</c:v>
+                  <c:v>42808</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42779</c:v>
+                  <c:v>42809</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42780</c:v>
+                  <c:v>42810</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42781</c:v>
+                  <c:v>42811</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42782</c:v>
+                  <c:v>42812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42783</c:v>
+                  <c:v>42813</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42784</c:v>
+                  <c:v>42814</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42785</c:v>
+                  <c:v>42815</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42786</c:v>
+                  <c:v>42816</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42787</c:v>
+                  <c:v>42817</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>42788</c:v>
+                  <c:v>42818</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42789</c:v>
+                  <c:v>42819</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>42790</c:v>
+                  <c:v>42820</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>42791</c:v>
+                  <c:v>42821</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>42792</c:v>
+                  <c:v>42822</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>42793</c:v>
+                  <c:v>42823</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>42794</c:v>
+                  <c:v>42824</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>42795</c:v>
+                  <c:v>42825</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>42796</c:v>
+                  <c:v>42826</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>42797</c:v>
+                  <c:v>42827</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>42798</c:v>
+                  <c:v>42828</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>42799</c:v>
+                  <c:v>42829</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>42800</c:v>
+                  <c:v>42830</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>42801</c:v>
+                  <c:v>42831</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>42802</c:v>
+                  <c:v>42832</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>42803</c:v>
+                  <c:v>42833</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>42804</c:v>
+                  <c:v>42834</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>42805</c:v>
+                  <c:v>42835</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>42806</c:v>
+                  <c:v>42836</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>42807</c:v>
+                  <c:v>42837</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>42808</c:v>
+                  <c:v>42838</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>42809</c:v>
+                  <c:v>42839</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>42810</c:v>
+                  <c:v>42840</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>42811</c:v>
+                  <c:v>42841</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>42812</c:v>
+                  <c:v>42842</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>42813</c:v>
+                  <c:v>42843</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>42814</c:v>
+                  <c:v>42844</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>42815</c:v>
+                  <c:v>42845</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>42816</c:v>
+                  <c:v>42846</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>42817</c:v>
+                  <c:v>42847</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>42818</c:v>
+                  <c:v>42848</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>42819</c:v>
+                  <c:v>42849</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>42820</c:v>
+                  <c:v>42850</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>42821</c:v>
+                  <c:v>42851</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>42822</c:v>
+                  <c:v>42852</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>42823</c:v>
+                  <c:v>42853</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>42824</c:v>
+                  <c:v>42854</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>42825</c:v>
+                  <c:v>42855</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>42826</c:v>
+                  <c:v>42856</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>42827</c:v>
+                  <c:v>42857</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>42828</c:v>
+                  <c:v>42858</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>42829</c:v>
+                  <c:v>42859</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>42830</c:v>
+                  <c:v>42860</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>42831</c:v>
+                  <c:v>42861</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>42832</c:v>
+                  <c:v>42862</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>42833</c:v>
+                  <c:v>42863</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>42834</c:v>
+                  <c:v>42864</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>42835</c:v>
+                  <c:v>42865</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>42836</c:v>
+                  <c:v>42866</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>42837</c:v>
+                  <c:v>42867</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>42838</c:v>
+                  <c:v>42868</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1270,199 +1267,199 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>3</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1513,199 +1510,199 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>42774</c:v>
+                  <c:v>42804</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42775</c:v>
+                  <c:v>42805</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42776</c:v>
+                  <c:v>42806</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42777</c:v>
+                  <c:v>42807</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42778</c:v>
+                  <c:v>42808</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42779</c:v>
+                  <c:v>42809</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42780</c:v>
+                  <c:v>42810</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42781</c:v>
+                  <c:v>42811</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42782</c:v>
+                  <c:v>42812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42783</c:v>
+                  <c:v>42813</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42784</c:v>
+                  <c:v>42814</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42785</c:v>
+                  <c:v>42815</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42786</c:v>
+                  <c:v>42816</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42787</c:v>
+                  <c:v>42817</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>42788</c:v>
+                  <c:v>42818</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42789</c:v>
+                  <c:v>42819</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>42790</c:v>
+                  <c:v>42820</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>42791</c:v>
+                  <c:v>42821</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>42792</c:v>
+                  <c:v>42822</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>42793</c:v>
+                  <c:v>42823</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>42794</c:v>
+                  <c:v>42824</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>42795</c:v>
+                  <c:v>42825</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>42796</c:v>
+                  <c:v>42826</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>42797</c:v>
+                  <c:v>42827</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>42798</c:v>
+                  <c:v>42828</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>42799</c:v>
+                  <c:v>42829</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>42800</c:v>
+                  <c:v>42830</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>42801</c:v>
+                  <c:v>42831</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>42802</c:v>
+                  <c:v>42832</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>42803</c:v>
+                  <c:v>42833</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>42804</c:v>
+                  <c:v>42834</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>42805</c:v>
+                  <c:v>42835</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>42806</c:v>
+                  <c:v>42836</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>42807</c:v>
+                  <c:v>42837</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>42808</c:v>
+                  <c:v>42838</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>42809</c:v>
+                  <c:v>42839</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>42810</c:v>
+                  <c:v>42840</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>42811</c:v>
+                  <c:v>42841</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>42812</c:v>
+                  <c:v>42842</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>42813</c:v>
+                  <c:v>42843</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>42814</c:v>
+                  <c:v>42844</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>42815</c:v>
+                  <c:v>42845</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>42816</c:v>
+                  <c:v>42846</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>42817</c:v>
+                  <c:v>42847</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>42818</c:v>
+                  <c:v>42848</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>42819</c:v>
+                  <c:v>42849</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>42820</c:v>
+                  <c:v>42850</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>42821</c:v>
+                  <c:v>42851</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>42822</c:v>
+                  <c:v>42852</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>42823</c:v>
+                  <c:v>42853</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>42824</c:v>
+                  <c:v>42854</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>42825</c:v>
+                  <c:v>42855</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>42826</c:v>
+                  <c:v>42856</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>42827</c:v>
+                  <c:v>42857</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>42828</c:v>
+                  <c:v>42858</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>42829</c:v>
+                  <c:v>42859</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>42830</c:v>
+                  <c:v>42860</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>42831</c:v>
+                  <c:v>42861</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>42832</c:v>
+                  <c:v>42862</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>42833</c:v>
+                  <c:v>42863</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>42834</c:v>
+                  <c:v>42864</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>42835</c:v>
+                  <c:v>42865</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>42836</c:v>
+                  <c:v>42866</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>42837</c:v>
+                  <c:v>42867</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>42838</c:v>
+                  <c:v>42868</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1717,199 +1714,199 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1995,199 +1992,199 @@
                 <c:formatCode>m/d/yyyy</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>42774</c:v>
+                  <c:v>42804</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>42775</c:v>
+                  <c:v>42805</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>42776</c:v>
+                  <c:v>42806</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>42777</c:v>
+                  <c:v>42807</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>42778</c:v>
+                  <c:v>42808</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>42779</c:v>
+                  <c:v>42809</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>42780</c:v>
+                  <c:v>42810</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42781</c:v>
+                  <c:v>42811</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>42782</c:v>
+                  <c:v>42812</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>42783</c:v>
+                  <c:v>42813</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>42784</c:v>
+                  <c:v>42814</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>42785</c:v>
+                  <c:v>42815</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>42786</c:v>
+                  <c:v>42816</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>42787</c:v>
+                  <c:v>42817</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>42788</c:v>
+                  <c:v>42818</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>42789</c:v>
+                  <c:v>42819</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>42790</c:v>
+                  <c:v>42820</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>42791</c:v>
+                  <c:v>42821</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>42792</c:v>
+                  <c:v>42822</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>42793</c:v>
+                  <c:v>42823</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>42794</c:v>
+                  <c:v>42824</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>42795</c:v>
+                  <c:v>42825</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>42796</c:v>
+                  <c:v>42826</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>42797</c:v>
+                  <c:v>42827</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>42798</c:v>
+                  <c:v>42828</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>42799</c:v>
+                  <c:v>42829</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>42800</c:v>
+                  <c:v>42830</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>42801</c:v>
+                  <c:v>42831</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>42802</c:v>
+                  <c:v>42832</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>42803</c:v>
+                  <c:v>42833</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>42804</c:v>
+                  <c:v>42834</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>42805</c:v>
+                  <c:v>42835</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>42806</c:v>
+                  <c:v>42836</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>42807</c:v>
+                  <c:v>42837</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>42808</c:v>
+                  <c:v>42838</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>42809</c:v>
+                  <c:v>42839</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>42810</c:v>
+                  <c:v>42840</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>42811</c:v>
+                  <c:v>42841</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>42812</c:v>
+                  <c:v>42842</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>42813</c:v>
+                  <c:v>42843</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>42814</c:v>
+                  <c:v>42844</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>42815</c:v>
+                  <c:v>42845</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>42816</c:v>
+                  <c:v>42846</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>42817</c:v>
+                  <c:v>42847</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>42818</c:v>
+                  <c:v>42848</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>42819</c:v>
+                  <c:v>42849</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>42820</c:v>
+                  <c:v>42850</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>42821</c:v>
+                  <c:v>42851</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>42822</c:v>
+                  <c:v>42852</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>42823</c:v>
+                  <c:v>42853</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>42824</c:v>
+                  <c:v>42854</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>42825</c:v>
+                  <c:v>42855</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>42826</c:v>
+                  <c:v>42856</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>42827</c:v>
+                  <c:v>42857</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>42828</c:v>
+                  <c:v>42858</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>42829</c:v>
+                  <c:v>42859</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>42830</c:v>
+                  <c:v>42860</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>42831</c:v>
+                  <c:v>42861</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>42832</c:v>
+                  <c:v>42862</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>42833</c:v>
+                  <c:v>42863</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>42834</c:v>
+                  <c:v>42864</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>42835</c:v>
+                  <c:v>42865</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>42836</c:v>
+                  <c:v>42866</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>42837</c:v>
+                  <c:v>42867</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>42838</c:v>
+                  <c:v>42868</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2199,274 +2196,274 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>3.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>3.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>3.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>3.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>3.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>3.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>3.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2552,274 +2549,274 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="90"/>
                 <c:pt idx="0">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>2.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2.12</c:v>
+                  <c:v>1.04</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>0.12</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2836,11 +2833,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="108931328"/>
-        <c:axId val="108941312"/>
+        <c:axId val="77420800"/>
+        <c:axId val="77434880"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="108931328"/>
+        <c:axId val="77420800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2888,14 +2885,14 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="108941312"/>
+        <c:crossAx val="77434880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="108941312"/>
+        <c:axId val="77434880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2905,7 +2902,7 @@
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="none"/>
-        <c:crossAx val="108931328"/>
+        <c:crossAx val="77420800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3914,7 +3911,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3928,8 +3925,8 @@
   </sheetPr>
   <dimension ref="B1:N201"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3994,7 +3991,7 @@
       </c>
       <c r="I3" s="7">
         <f ca="1">TODAY()</f>
-        <v>42863</v>
+        <v>42893</v>
       </c>
       <c r="J3" s="8">
         <v>90</v>
@@ -4208,10 +4205,10 @@
         <v>3</v>
       </c>
       <c r="C20" s="21" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>58</v>
+        <v>36</v>
       </c>
       <c r="E20" s="22" t="s">
         <v>30</v>
@@ -4229,7 +4226,7 @@
         <v>54</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="2:14" ht="15.75" x14ac:dyDescent="0.25">
@@ -5111,7 +5108,7 @@
       </c>
       <c r="J8" s="1">
         <f ca="1">'Issue Tracker'!I3</f>
-        <v>42863</v>
+        <v>42893</v>
       </c>
       <c r="N8">
         <f ca="1">COUNT(typesUnsorted)</f>
@@ -5199,15 +5196,15 @@
       </c>
       <c r="H16" s="1">
         <f t="shared" ref="H16:H47" ca="1" si="0">keydate-days+G16</f>
-        <v>42774</v>
+        <v>42804</v>
       </c>
       <c r="I16">
         <f ca="1">I15+COUNTIFS(issues[OPENED ON],H16,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J16">
         <f ca="1">J15+COUNTIFS(issues[CLOSED ON],H16,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N16" t="str">
         <f t="array" ref="N16">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N15, issues[TYPE]),0))</f>
@@ -5232,19 +5229,19 @@
       </c>
       <c r="H17" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42775</v>
+        <v>42805</v>
       </c>
       <c r="I17">
         <f ca="1">I16+COUNTIFS(issues[OPENED ON],H17,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J17">
         <f ca="1">J16+COUNTIFS(issues[CLOSED ON],H17,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N17" t="str">
         <f t="array" ref="N17">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N16, issues[TYPE]),0))</f>
-        <v>Relibilirt</v>
+        <v>Reliability</v>
       </c>
       <c r="O17" t="str">
         <f t="array" ref="O17">INDEX(issues[PRIORITY],MATCH(0,COUNTIF(O$15:O16,issues[PRIORITY]),0))</f>
@@ -5265,15 +5262,15 @@
       </c>
       <c r="H18" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42776</v>
+        <v>42806</v>
       </c>
       <c r="I18">
         <f ca="1">I17+COUNTIFS(issues[OPENED ON],H18,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J18">
         <f ca="1">J17+COUNTIFS(issues[CLOSED ON],H18,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N18">
         <f t="array" ref="N18">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N17, issues[TYPE]),0))</f>
@@ -5285,7 +5282,7 @@
       </c>
       <c r="S18" t="str">
         <f t="array" aca="1" ref="S18" ca="1">INDEX(typesUnsorted, MATCH(SMALL(COUNTIF(typesUnsorted, "&lt;"&amp;typesUnsorted), ROW(3:3)), COUNTIF(typesUnsorted, "&lt;"&amp;typesUnsorted), 0))</f>
-        <v>Relibilirt</v>
+        <v>Reliability</v>
       </c>
       <c r="T18" t="str">
         <f t="array" aca="1" ref="T18" ca="1">INDEX(prioritiesUnsorted, MATCH(SMALL(COUNTIF(prioritiesUnsorted, "&lt;"&amp;prioritiesUnsorted), ROW(3:3)), COUNTIF(prioritiesUnsorted, "&lt;"&amp;prioritiesUnsorted), 0))</f>
@@ -5298,15 +5295,15 @@
       </c>
       <c r="H19" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42777</v>
+        <v>42807</v>
       </c>
       <c r="I19">
         <f ca="1">I18+COUNTIFS(issues[OPENED ON],H19,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J19">
         <f ca="1">J18+COUNTIFS(issues[CLOSED ON],H19,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N19" t="e">
         <f t="array" ref="N19">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N18, issues[TYPE]),0))</f>
@@ -5331,15 +5328,15 @@
       </c>
       <c r="H20" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42778</v>
+        <v>42808</v>
       </c>
       <c r="I20">
         <f ca="1">I19+COUNTIFS(issues[OPENED ON],H20,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J20">
         <f ca="1">J19+COUNTIFS(issues[CLOSED ON],H20,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N20" t="e">
         <f t="array" ref="N20">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N19, issues[TYPE]),0))</f>
@@ -5364,15 +5361,15 @@
       </c>
       <c r="H21" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42779</v>
+        <v>42809</v>
       </c>
       <c r="I21">
         <f ca="1">I20+COUNTIFS(issues[OPENED ON],H21,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J21">
         <f ca="1">J20+COUNTIFS(issues[CLOSED ON],H21,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N21" t="e">
         <f t="array" ref="N21">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N20, issues[TYPE]),0))</f>
@@ -5397,15 +5394,15 @@
       </c>
       <c r="H22" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42780</v>
+        <v>42810</v>
       </c>
       <c r="I22">
         <f ca="1">I21+COUNTIFS(issues[OPENED ON],H22,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J22">
         <f ca="1">J21+COUNTIFS(issues[CLOSED ON],H22,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N22" t="e">
         <f t="array" ref="N22">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N21, issues[TYPE]),0))</f>
@@ -5430,15 +5427,15 @@
       </c>
       <c r="H23" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42781</v>
+        <v>42811</v>
       </c>
       <c r="I23">
         <f ca="1">I22+COUNTIFS(issues[OPENED ON],H23,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J23">
         <f ca="1">J22+COUNTIFS(issues[CLOSED ON],H23,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N23" t="e">
         <f t="array" ref="N23">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N22, issues[TYPE]),0))</f>
@@ -5463,15 +5460,15 @@
       </c>
       <c r="H24" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42782</v>
+        <v>42812</v>
       </c>
       <c r="I24">
         <f ca="1">I23+COUNTIFS(issues[OPENED ON],H24,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J24">
         <f ca="1">J23+COUNTIFS(issues[CLOSED ON],H24,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N24" t="e">
         <f t="array" ref="N24">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N23, issues[TYPE]),0))</f>
@@ -5496,15 +5493,15 @@
       </c>
       <c r="H25" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42783</v>
+        <v>42813</v>
       </c>
       <c r="I25">
         <f ca="1">I24+COUNTIFS(issues[OPENED ON],H25,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J25">
         <f ca="1">J24+COUNTIFS(issues[CLOSED ON],H25,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N25" t="e">
         <f t="array" ref="N25">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N24, issues[TYPE]),0))</f>
@@ -5529,15 +5526,15 @@
       </c>
       <c r="H26" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42784</v>
+        <v>42814</v>
       </c>
       <c r="I26">
         <f ca="1">I25+COUNTIFS(issues[OPENED ON],H26,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J26">
         <f ca="1">J25+COUNTIFS(issues[CLOSED ON],H26,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N26" t="e">
         <f t="array" ref="N26">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N25, issues[TYPE]),0))</f>
@@ -5562,15 +5559,15 @@
       </c>
       <c r="H27" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42785</v>
+        <v>42815</v>
       </c>
       <c r="I27">
         <f ca="1">I26+COUNTIFS(issues[OPENED ON],H27,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J27">
         <f ca="1">J26+COUNTIFS(issues[CLOSED ON],H27,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N27" t="e">
         <f t="array" ref="N27">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N26, issues[TYPE]),0))</f>
@@ -5595,15 +5592,15 @@
       </c>
       <c r="H28" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42786</v>
+        <v>42816</v>
       </c>
       <c r="I28">
         <f ca="1">I27+COUNTIFS(issues[OPENED ON],H28,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J28">
         <f ca="1">J27+COUNTIFS(issues[CLOSED ON],H28,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N28" t="e">
         <f t="array" ref="N28">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N27, issues[TYPE]),0))</f>
@@ -5628,15 +5625,15 @@
       </c>
       <c r="H29" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42787</v>
+        <v>42817</v>
       </c>
       <c r="I29">
         <f ca="1">I28+COUNTIFS(issues[OPENED ON],H29,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J29">
         <f ca="1">J28+COUNTIFS(issues[CLOSED ON],H29,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N29" t="e">
         <f t="array" ref="N29">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N28, issues[TYPE]),0))</f>
@@ -5661,15 +5658,15 @@
       </c>
       <c r="H30" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42788</v>
+        <v>42818</v>
       </c>
       <c r="I30">
         <f ca="1">I29+COUNTIFS(issues[OPENED ON],H30,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J30">
         <f ca="1">J29+COUNTIFS(issues[CLOSED ON],H30,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N30" t="e">
         <f t="array" ref="N30">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N29, issues[TYPE]),0))</f>
@@ -5694,15 +5691,15 @@
       </c>
       <c r="H31" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42789</v>
+        <v>42819</v>
       </c>
       <c r="I31">
         <f ca="1">I30+COUNTIFS(issues[OPENED ON],H31,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J31">
         <f ca="1">J30+COUNTIFS(issues[CLOSED ON],H31,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N31" t="e">
         <f t="array" ref="N31">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N30, issues[TYPE]),0))</f>
@@ -5727,15 +5724,15 @@
       </c>
       <c r="H32" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42790</v>
+        <v>42820</v>
       </c>
       <c r="I32">
         <f ca="1">I31+COUNTIFS(issues[OPENED ON],H32,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J32">
         <f ca="1">J31+COUNTIFS(issues[CLOSED ON],H32,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N32" t="e">
         <f t="array" ref="N32">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N31, issues[TYPE]),0))</f>
@@ -5760,15 +5757,15 @@
       </c>
       <c r="H33" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42791</v>
+        <v>42821</v>
       </c>
       <c r="I33">
         <f ca="1">I32+COUNTIFS(issues[OPENED ON],H33,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J33">
         <f ca="1">J32+COUNTIFS(issues[CLOSED ON],H33,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N33" t="e">
         <f t="array" ref="N33">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N32, issues[TYPE]),0))</f>
@@ -5793,15 +5790,15 @@
       </c>
       <c r="H34" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42792</v>
+        <v>42822</v>
       </c>
       <c r="I34">
         <f ca="1">I33+COUNTIFS(issues[OPENED ON],H34,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J34">
         <f ca="1">J33+COUNTIFS(issues[CLOSED ON],H34,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N34" t="e">
         <f t="array" ref="N34">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N33, issues[TYPE]),0))</f>
@@ -5826,15 +5823,15 @@
       </c>
       <c r="H35" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42793</v>
+        <v>42823</v>
       </c>
       <c r="I35">
         <f ca="1">I34+COUNTIFS(issues[OPENED ON],H35,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J35">
         <f ca="1">J34+COUNTIFS(issues[CLOSED ON],H35,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N35" t="e">
         <f t="array" ref="N35">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N34, issues[TYPE]),0))</f>
@@ -5859,15 +5856,15 @@
       </c>
       <c r="H36" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42794</v>
+        <v>42824</v>
       </c>
       <c r="I36">
         <f ca="1">I35+COUNTIFS(issues[OPENED ON],H36,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J36">
         <f ca="1">J35+COUNTIFS(issues[CLOSED ON],H36,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N36" t="e">
         <f t="array" ref="N36">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N35, issues[TYPE]),0))</f>
@@ -5892,15 +5889,15 @@
       </c>
       <c r="H37" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42795</v>
+        <v>42825</v>
       </c>
       <c r="I37">
         <f ca="1">I36+COUNTIFS(issues[OPENED ON],H37,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J37">
         <f ca="1">J36+COUNTIFS(issues[CLOSED ON],H37,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N37" t="e">
         <f t="array" ref="N37">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N36, issues[TYPE]),0))</f>
@@ -5925,15 +5922,15 @@
       </c>
       <c r="H38" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42796</v>
+        <v>42826</v>
       </c>
       <c r="I38">
         <f ca="1">I37+COUNTIFS(issues[OPENED ON],H38,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J38">
         <f ca="1">J37+COUNTIFS(issues[CLOSED ON],H38,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N38" t="e">
         <f t="array" ref="N38">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N37, issues[TYPE]),0))</f>
@@ -5958,15 +5955,15 @@
       </c>
       <c r="H39" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42797</v>
+        <v>42827</v>
       </c>
       <c r="I39">
         <f ca="1">I38+COUNTIFS(issues[OPENED ON],H39,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J39">
         <f ca="1">J38+COUNTIFS(issues[CLOSED ON],H39,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N39" t="e">
         <f t="array" ref="N39">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N38, issues[TYPE]),0))</f>
@@ -5991,15 +5988,15 @@
       </c>
       <c r="H40" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42798</v>
+        <v>42828</v>
       </c>
       <c r="I40">
         <f ca="1">I39+COUNTIFS(issues[OPENED ON],H40,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J40">
         <f ca="1">J39+COUNTIFS(issues[CLOSED ON],H40,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N40" t="e">
         <f t="array" ref="N40">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N39, issues[TYPE]),0))</f>
@@ -6024,15 +6021,15 @@
       </c>
       <c r="H41" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42799</v>
+        <v>42829</v>
       </c>
       <c r="I41">
         <f ca="1">I40+COUNTIFS(issues[OPENED ON],H41,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J41">
         <f ca="1">J40+COUNTIFS(issues[CLOSED ON],H41,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N41" t="e">
         <f t="array" ref="N41">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N40, issues[TYPE]),0))</f>
@@ -6057,15 +6054,15 @@
       </c>
       <c r="H42" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42800</v>
+        <v>42830</v>
       </c>
       <c r="I42">
         <f ca="1">I41+COUNTIFS(issues[OPENED ON],H42,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J42">
         <f ca="1">J41+COUNTIFS(issues[CLOSED ON],H42,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N42" t="e">
         <f t="array" ref="N42">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N41, issues[TYPE]),0))</f>
@@ -6090,15 +6087,15 @@
       </c>
       <c r="H43" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42801</v>
+        <v>42831</v>
       </c>
       <c r="I43">
         <f ca="1">I42+COUNTIFS(issues[OPENED ON],H43,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J43">
         <f ca="1">J42+COUNTIFS(issues[CLOSED ON],H43,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N43" t="e">
         <f t="array" ref="N43">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N42, issues[TYPE]),0))</f>
@@ -6123,15 +6120,15 @@
       </c>
       <c r="H44" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42802</v>
+        <v>42832</v>
       </c>
       <c r="I44">
         <f ca="1">I43+COUNTIFS(issues[OPENED ON],H44,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J44">
         <f ca="1">J43+COUNTIFS(issues[CLOSED ON],H44,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N44" t="e">
         <f t="array" ref="N44">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N43, issues[TYPE]),0))</f>
@@ -6156,15 +6153,15 @@
       </c>
       <c r="H45" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42803</v>
+        <v>42833</v>
       </c>
       <c r="I45">
         <f ca="1">I44+COUNTIFS(issues[OPENED ON],H45,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J45">
         <f ca="1">J44+COUNTIFS(issues[CLOSED ON],H45,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="N45" t="e">
         <f t="array" ref="N45">INDEX(issues[TYPE],MATCH(0,COUNTIF(N$15:N44, issues[TYPE]),0))</f>
@@ -6189,15 +6186,15 @@
       </c>
       <c r="H46" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42804</v>
+        <v>42834</v>
       </c>
       <c r="I46">
         <f ca="1">I45+COUNTIFS(issues[OPENED ON],H46,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J46">
         <f ca="1">J45+COUNTIFS(issues[CLOSED ON],H46,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="7:20" x14ac:dyDescent="0.25">
@@ -6206,15 +6203,15 @@
       </c>
       <c r="H47" s="1">
         <f t="shared" ca="1" si="0"/>
-        <v>42805</v>
+        <v>42835</v>
       </c>
       <c r="I47">
         <f ca="1">I46+COUNTIFS(issues[OPENED ON],H47,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J47">
         <f ca="1">J46+COUNTIFS(issues[CLOSED ON],H47,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="7:20" x14ac:dyDescent="0.25">
@@ -6223,15 +6220,15 @@
       </c>
       <c r="H48" s="1">
         <f t="shared" ref="H48:H79" ca="1" si="1">keydate-days+G48</f>
-        <v>42806</v>
+        <v>42836</v>
       </c>
       <c r="I48">
         <f ca="1">I47+COUNTIFS(issues[OPENED ON],H48,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J48">
         <f ca="1">J47+COUNTIFS(issues[CLOSED ON],H48,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="7:10" x14ac:dyDescent="0.25">
@@ -6240,15 +6237,15 @@
       </c>
       <c r="H49" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42807</v>
+        <v>42837</v>
       </c>
       <c r="I49">
         <f ca="1">I48+COUNTIFS(issues[OPENED ON],H49,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J49">
         <f ca="1">J48+COUNTIFS(issues[CLOSED ON],H49,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="7:10" x14ac:dyDescent="0.25">
@@ -6257,15 +6254,15 @@
       </c>
       <c r="H50" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42808</v>
+        <v>42838</v>
       </c>
       <c r="I50">
         <f ca="1">I49+COUNTIFS(issues[OPENED ON],H50,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J50">
         <f ca="1">J49+COUNTIFS(issues[CLOSED ON],H50,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="7:10" x14ac:dyDescent="0.25">
@@ -6274,15 +6271,15 @@
       </c>
       <c r="H51" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42809</v>
+        <v>42839</v>
       </c>
       <c r="I51">
         <f ca="1">I50+COUNTIFS(issues[OPENED ON],H51,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J51">
         <f ca="1">J50+COUNTIFS(issues[CLOSED ON],H51,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="7:10" x14ac:dyDescent="0.25">
@@ -6291,15 +6288,15 @@
       </c>
       <c r="H52" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42810</v>
+        <v>42840</v>
       </c>
       <c r="I52">
         <f ca="1">I51+COUNTIFS(issues[OPENED ON],H52,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J52">
         <f ca="1">J51+COUNTIFS(issues[CLOSED ON],H52,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="7:10" x14ac:dyDescent="0.25">
@@ -6308,15 +6305,15 @@
       </c>
       <c r="H53" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42811</v>
+        <v>42841</v>
       </c>
       <c r="I53">
         <f ca="1">I52+COUNTIFS(issues[OPENED ON],H53,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J53">
         <f ca="1">J52+COUNTIFS(issues[CLOSED ON],H53,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="7:10" x14ac:dyDescent="0.25">
@@ -6325,15 +6322,15 @@
       </c>
       <c r="H54" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42812</v>
+        <v>42842</v>
       </c>
       <c r="I54">
         <f ca="1">I53+COUNTIFS(issues[OPENED ON],H54,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J54">
         <f ca="1">J53+COUNTIFS(issues[CLOSED ON],H54,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="7:10" x14ac:dyDescent="0.25">
@@ -6342,15 +6339,15 @@
       </c>
       <c r="H55" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42813</v>
+        <v>42843</v>
       </c>
       <c r="I55">
         <f ca="1">I54+COUNTIFS(issues[OPENED ON],H55,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J55">
         <f ca="1">J54+COUNTIFS(issues[CLOSED ON],H55,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="7:10" x14ac:dyDescent="0.25">
@@ -6359,15 +6356,15 @@
       </c>
       <c r="H56" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42814</v>
+        <v>42844</v>
       </c>
       <c r="I56">
         <f ca="1">I55+COUNTIFS(issues[OPENED ON],H56,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J56">
         <f ca="1">J55+COUNTIFS(issues[CLOSED ON],H56,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="7:10" x14ac:dyDescent="0.25">
@@ -6376,15 +6373,15 @@
       </c>
       <c r="H57" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42815</v>
+        <v>42845</v>
       </c>
       <c r="I57">
         <f ca="1">I56+COUNTIFS(issues[OPENED ON],H57,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J57">
         <f ca="1">J56+COUNTIFS(issues[CLOSED ON],H57,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="7:10" x14ac:dyDescent="0.25">
@@ -6393,15 +6390,15 @@
       </c>
       <c r="H58" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42816</v>
+        <v>42846</v>
       </c>
       <c r="I58">
         <f ca="1">I57+COUNTIFS(issues[OPENED ON],H58,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J58">
         <f ca="1">J57+COUNTIFS(issues[CLOSED ON],H58,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="7:10" x14ac:dyDescent="0.25">
@@ -6410,15 +6407,15 @@
       </c>
       <c r="H59" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42817</v>
+        <v>42847</v>
       </c>
       <c r="I59">
         <f ca="1">I58+COUNTIFS(issues[OPENED ON],H59,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J59">
         <f ca="1">J58+COUNTIFS(issues[CLOSED ON],H59,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="7:10" x14ac:dyDescent="0.25">
@@ -6427,15 +6424,15 @@
       </c>
       <c r="H60" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42818</v>
+        <v>42848</v>
       </c>
       <c r="I60">
         <f ca="1">I59+COUNTIFS(issues[OPENED ON],H60,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J60">
         <f ca="1">J59+COUNTIFS(issues[CLOSED ON],H60,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="7:10" x14ac:dyDescent="0.25">
@@ -6444,15 +6441,15 @@
       </c>
       <c r="H61" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42819</v>
+        <v>42849</v>
       </c>
       <c r="I61">
         <f ca="1">I60+COUNTIFS(issues[OPENED ON],H61,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J61">
         <f ca="1">J60+COUNTIFS(issues[CLOSED ON],H61,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="7:10" x14ac:dyDescent="0.25">
@@ -6461,15 +6458,15 @@
       </c>
       <c r="H62" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42820</v>
+        <v>42850</v>
       </c>
       <c r="I62">
         <f ca="1">I61+COUNTIFS(issues[OPENED ON],H62,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J62">
         <f ca="1">J61+COUNTIFS(issues[CLOSED ON],H62,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="7:10" x14ac:dyDescent="0.25">
@@ -6478,15 +6475,15 @@
       </c>
       <c r="H63" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42821</v>
+        <v>42851</v>
       </c>
       <c r="I63">
         <f ca="1">I62+COUNTIFS(issues[OPENED ON],H63,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J63">
         <f ca="1">J62+COUNTIFS(issues[CLOSED ON],H63,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="64" spans="7:10" x14ac:dyDescent="0.25">
@@ -6495,15 +6492,15 @@
       </c>
       <c r="H64" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42822</v>
+        <v>42852</v>
       </c>
       <c r="I64">
         <f ca="1">I63+COUNTIFS(issues[OPENED ON],H64,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J64">
         <f ca="1">J63+COUNTIFS(issues[CLOSED ON],H64,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" spans="7:10" x14ac:dyDescent="0.25">
@@ -6512,15 +6509,15 @@
       </c>
       <c r="H65" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42823</v>
+        <v>42853</v>
       </c>
       <c r="I65">
         <f ca="1">I64+COUNTIFS(issues[OPENED ON],H65,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J65">
         <f ca="1">J64+COUNTIFS(issues[CLOSED ON],H65,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="66" spans="7:10" x14ac:dyDescent="0.25">
@@ -6529,15 +6526,15 @@
       </c>
       <c r="H66" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42824</v>
+        <v>42854</v>
       </c>
       <c r="I66">
         <f ca="1">I65+COUNTIFS(issues[OPENED ON],H66,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J66">
         <f ca="1">J65+COUNTIFS(issues[CLOSED ON],H66,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="67" spans="7:10" x14ac:dyDescent="0.25">
@@ -6546,15 +6543,15 @@
       </c>
       <c r="H67" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42825</v>
+        <v>42855</v>
       </c>
       <c r="I67">
         <f ca="1">I66+COUNTIFS(issues[OPENED ON],H67,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J67">
         <f ca="1">J66+COUNTIFS(issues[CLOSED ON],H67,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68" spans="7:10" x14ac:dyDescent="0.25">
@@ -6563,15 +6560,15 @@
       </c>
       <c r="H68" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42826</v>
+        <v>42856</v>
       </c>
       <c r="I68">
         <f ca="1">I67+COUNTIFS(issues[OPENED ON],H68,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J68">
         <f ca="1">J67+COUNTIFS(issues[CLOSED ON],H68,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="69" spans="7:10" x14ac:dyDescent="0.25">
@@ -6580,15 +6577,15 @@
       </c>
       <c r="H69" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42827</v>
+        <v>42857</v>
       </c>
       <c r="I69">
         <f ca="1">I68+COUNTIFS(issues[OPENED ON],H69,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J69">
         <f ca="1">J68+COUNTIFS(issues[CLOSED ON],H69,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" spans="7:10" x14ac:dyDescent="0.25">
@@ -6597,15 +6594,15 @@
       </c>
       <c r="H70" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42828</v>
+        <v>42858</v>
       </c>
       <c r="I70">
         <f ca="1">I69+COUNTIFS(issues[OPENED ON],H70,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J70">
         <f ca="1">J69+COUNTIFS(issues[CLOSED ON],H70,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71" spans="7:10" x14ac:dyDescent="0.25">
@@ -6614,15 +6611,15 @@
       </c>
       <c r="H71" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42829</v>
+        <v>42859</v>
       </c>
       <c r="I71">
         <f ca="1">I70+COUNTIFS(issues[OPENED ON],H71,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J71">
         <f ca="1">J70+COUNTIFS(issues[CLOSED ON],H71,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="7:10" x14ac:dyDescent="0.25">
@@ -6631,15 +6628,15 @@
       </c>
       <c r="H72" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42830</v>
+        <v>42860</v>
       </c>
       <c r="I72">
         <f ca="1">I71+COUNTIFS(issues[OPENED ON],H72,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J72">
         <f ca="1">J71+COUNTIFS(issues[CLOSED ON],H72,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="73" spans="7:10" x14ac:dyDescent="0.25">
@@ -6648,15 +6645,15 @@
       </c>
       <c r="H73" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42831</v>
+        <v>42861</v>
       </c>
       <c r="I73">
         <f ca="1">I72+COUNTIFS(issues[OPENED ON],H73,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J73">
         <f ca="1">J72+COUNTIFS(issues[CLOSED ON],H73,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="74" spans="7:10" x14ac:dyDescent="0.25">
@@ -6665,15 +6662,15 @@
       </c>
       <c r="H74" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42832</v>
+        <v>42862</v>
       </c>
       <c r="I74">
         <f ca="1">I73+COUNTIFS(issues[OPENED ON],H74,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J74">
         <f ca="1">J73+COUNTIFS(issues[CLOSED ON],H74,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="7:10" x14ac:dyDescent="0.25">
@@ -6682,15 +6679,15 @@
       </c>
       <c r="H75" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42833</v>
+        <v>42863</v>
       </c>
       <c r="I75">
         <f ca="1">I74+COUNTIFS(issues[OPENED ON],H75,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J75">
         <f ca="1">J74+COUNTIFS(issues[CLOSED ON],H75,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="7:10" x14ac:dyDescent="0.25">
@@ -6699,15 +6696,15 @@
       </c>
       <c r="H76" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42834</v>
+        <v>42864</v>
       </c>
       <c r="I76">
         <f ca="1">I75+COUNTIFS(issues[OPENED ON],H76,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J76">
         <f ca="1">J75+COUNTIFS(issues[CLOSED ON],H76,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="7:10" x14ac:dyDescent="0.25">
@@ -6716,15 +6713,15 @@
       </c>
       <c r="H77" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42835</v>
+        <v>42865</v>
       </c>
       <c r="I77">
         <f ca="1">I76+COUNTIFS(issues[OPENED ON],H77,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J77">
         <f ca="1">J76+COUNTIFS(issues[CLOSED ON],H77,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78" spans="7:10" x14ac:dyDescent="0.25">
@@ -6733,15 +6730,15 @@
       </c>
       <c r="H78" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42836</v>
+        <v>42866</v>
       </c>
       <c r="I78">
         <f ca="1">I77+COUNTIFS(issues[OPENED ON],H78,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J78">
         <f ca="1">J77+COUNTIFS(issues[CLOSED ON],H78,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="7:10" x14ac:dyDescent="0.25">
@@ -6750,15 +6747,15 @@
       </c>
       <c r="H79" s="1">
         <f t="shared" ca="1" si="1"/>
-        <v>42837</v>
+        <v>42867</v>
       </c>
       <c r="I79">
         <f ca="1">I78+COUNTIFS(issues[OPENED ON],H79,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J79">
         <f ca="1">J78+COUNTIFS(issues[CLOSED ON],H79,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="80" spans="7:10" x14ac:dyDescent="0.25">
@@ -6767,15 +6764,15 @@
       </c>
       <c r="H80" s="1">
         <f t="shared" ref="H80" ca="1" si="2">keydate-days+G80</f>
-        <v>42838</v>
+        <v>42868</v>
       </c>
       <c r="I80">
         <f ca="1">I79+COUNTIFS(issues[OPENED ON],H80,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J80">
         <f ca="1">J79+COUNTIFS(issues[CLOSED ON],H80,issues[TYPE],type,issues[PRIORITY],priority)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>